<commit_message>
Analytics python routine and output file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/Drive-Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42905C5A-8D20-3647-8D07-A3147232A8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42580CCA-9101-324B-8913-5722EFE2AF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,7 +578,7 @@
   </sheetPr>
   <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView topLeftCell="J1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17436,7 +17436,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>